<commit_message>
moving old data to new directory for cleaner directory
</commit_message>
<xml_diff>
--- a/data/ivsc_3cmtct_shed3_param.xlsx
+++ b/data/ivsc_3cmtct_shed3_param.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/svn/BiologicsWorkstream/Work/010_Tissue_Concentration_Prediction/pgm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astein/Github/TumorModelingCode/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="460" windowWidth="24700" windowHeight="16840" tabRatio="500"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="24700" windowHeight="14960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="129">
   <si>
     <t>Parameter</t>
   </si>
@@ -189,15 +189,9 @@
     <t>From PopPK - exp(logV1)</t>
   </si>
   <si>
-    <t>Detail</t>
-  </si>
-  <si>
     <t>From PopPK - exp(logV2)</t>
   </si>
   <si>
-    <t>This number is really questionable.  Probably think a bit more</t>
-  </si>
-  <si>
     <t>Same as VD1</t>
   </si>
   <si>
@@ -246,9 +240,6 @@
     <t>From TMDD ~ exp(log(Kd))</t>
   </si>
   <si>
-    <t>From Table 4-1 of IB v2 (p17), converted to days</t>
-  </si>
-  <si>
     <t>Same as koff1</t>
   </si>
   <si>
@@ -276,9 +267,6 @@
     <t>Same as keD1</t>
   </si>
   <si>
-    <t>From KarthikSubra Slidedeck, slide 16 (log(2)/t1/2 h)*24</t>
-  </si>
-  <si>
     <t>TMDD-Shedding</t>
   </si>
   <si>
@@ -324,9 +312,6 @@
     <t xml:space="preserve">Ignore elimination from tumor - see Chen16 for justification.  </t>
   </si>
   <si>
-    <t>Li04 Fig3e: thalf = 5.4h, kshedM3 = log(2)/5.4h*24</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -442,12 +427,6 @@
   </si>
   <si>
     <t>From xxx</t>
-  </si>
-  <si>
-    <t>Work/001_Karthik_Varun/POPPK-2_Karthik/NONMEM/run13.lst</t>
-  </si>
-  <si>
-    <t>Work/001_Karthik_Varun/POPPK-2_Karthik/NONMEM/run9.lst</t>
   </si>
   <si>
     <t>Chosen to match the target accumulation.  
@@ -972,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,22 +967,21 @@
     <col min="6" max="6" width="7.83203125" style="6" customWidth="1"/>
     <col min="7" max="8" width="9.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="68.83203125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" style="10" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="10"/>
+    <col min="10" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1015,27 +993,24 @@
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
@@ -1053,18 +1028,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>7</v>
@@ -1082,48 +1057,48 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4" s="6">
         <f>EXP(-4.552)*24</f>
         <v>0.25310618628986775</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>13</v>
@@ -1136,54 +1111,54 @@
         <v>4</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F6" s="6">
         <f>EXP(-3.771)*24</f>
         <v>0.55269654590709449</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>21</v>
@@ -1196,27 +1171,24 @@
         <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I7" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>22</v>
@@ -1229,24 +1201,24 @@
         <v>2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>24</v>
@@ -1259,24 +1231,24 @@
         <v>2</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>26</v>
@@ -1289,24 +1261,24 @@
         <v>2</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>9</v>
@@ -1319,24 +1291,24 @@
         <v>4</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>10</v>
@@ -1349,82 +1321,79 @@
         <v>4</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15"/>
       <c r="B13" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F13" s="6">
         <v>57</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="16" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>12</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14" s="6">
         <f>EXP(1.22)</f>
         <v>3.3871877336213347</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>13</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>16</v>
@@ -1437,24 +1406,22 @@
         <v>4</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>14</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>18</v>
@@ -1467,24 +1434,24 @@
         <v>4</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>15</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>15</v>
@@ -1497,24 +1464,24 @@
         <v>20</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>17</v>
@@ -1527,22 +1494,22 @@
         <v>20</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>17</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>32</v>
@@ -1555,27 +1522,22 @@
         <v>4</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>18</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>34</v>
@@ -1588,24 +1550,24 @@
         <v>4</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>19</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>36</v>
@@ -1620,21 +1582,21 @@
         <v>0</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>20</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>37</v>
@@ -1649,21 +1611,21 @@
         <v>0</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="20" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="20" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>21</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>38</v>
@@ -1678,24 +1640,21 @@
         <v>1</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="J23" s="20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>22</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>39</v>
@@ -1708,24 +1667,22 @@
         <v>4</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>23</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>40</v>
@@ -1738,24 +1695,24 @@
         <v>4</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>24</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>23</v>
@@ -1767,27 +1724,24 @@
         <v>2</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="J26" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>25</v>
@@ -1800,24 +1754,24 @@
         <v>2</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>27</v>
@@ -1830,24 +1784,24 @@
         <v>2</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>14</v>
@@ -1862,21 +1816,21 @@
         <v>0</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>33</v>
@@ -1891,21 +1845,21 @@
         <v>0</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
         <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>35</v>
@@ -1920,21 +1874,21 @@
         <v>0</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
         <v>30</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>41</v>
@@ -1949,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -1957,13 +1911,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>42</v>
@@ -1978,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -1986,16 +1940,16 @@
         <v>32</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D34" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="F34" s="6">
         <v>0.3</v>
@@ -2004,10 +1958,10 @@
         <v>3</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -2015,16 +1969,16 @@
         <v>33</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F35" s="6">
         <v>0.4</v>
@@ -2033,10 +1987,10 @@
         <v>3</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2044,13 +1998,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>11</v>
@@ -2063,10 +2017,10 @@
         <v>4</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2074,13 +2028,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>28</v>
@@ -2093,10 +2047,10 @@
         <v>4</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2104,13 +2058,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>30</v>
@@ -2123,10 +2077,10 @@
         <v>4</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2134,13 +2088,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>12</v>
@@ -2153,10 +2107,10 @@
         <v>4</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2164,13 +2118,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>29</v>
@@ -2183,10 +2137,10 @@
         <v>4</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2194,13 +2148,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>31</v>
@@ -2213,10 +2167,10 @@
         <v>4</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>